<commit_message>
ready for final model
</commit_message>
<xml_diff>
--- a/src/experiments/results/main.xlsx
+++ b/src/experiments/results/main.xlsx
@@ -1341,23 +1341,23 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>POINT (7.043315311922979 49.30600054426942)</t>
+          <t>POINT (6.9355980807587105 49.364007303777186)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10041</v>
+        <v>10043</v>
       </c>
       <c r="C30" t="n">
-        <v>687653890</v>
+        <v>364882131</v>
       </c>
       <c r="D30" t="n">
         <v>300</v>
       </c>
       <c r="E30" t="n">
-        <v>49.30600054426942</v>
+        <v>49.36400730377719</v>
       </c>
       <c r="F30" t="n">
-        <v>7.043315311922979</v>
+        <v>6.935598080758711</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1368,23 +1368,23 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>POINT (6.9355980807587105 49.364007303777186)</t>
+          <t>POINT (7.001045558866386 49.401271550367575)</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>10043</v>
       </c>
       <c r="C31" t="n">
-        <v>364882131</v>
+        <v>419910303</v>
       </c>
       <c r="D31" t="n">
         <v>300</v>
       </c>
       <c r="E31" t="n">
-        <v>49.36400730377719</v>
+        <v>49.40127155036758</v>
       </c>
       <c r="F31" t="n">
-        <v>6.935598080758711</v>
+        <v>7.001045558866386</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1395,23 +1395,23 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>POINT (6.950952603408715 49.33048315182436)</t>
+          <t>POINT (7.029496440077044 49.403660960617195)</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>10043</v>
       </c>
       <c r="C32" t="n">
-        <v>264365825</v>
+        <v>388230747</v>
       </c>
       <c r="D32" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E32" t="n">
-        <v>49.33048315182436</v>
+        <v>49.4036609606172</v>
       </c>
       <c r="F32" t="n">
-        <v>6.950952603408715</v>
+        <v>7.029496440077044</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1422,23 +1422,23 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>POINT (7.029496440077044 49.403660960617195)</t>
+          <t>POINT (7.091227930374576 49.38422368213677)</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>10043</v>
       </c>
       <c r="C33" t="n">
-        <v>388230747</v>
+        <v>1264098455</v>
       </c>
       <c r="D33" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E33" t="n">
-        <v>49.4036609606172</v>
+        <v>49.38422368213677</v>
       </c>
       <c r="F33" t="n">
-        <v>7.029496440077044</v>
+        <v>7.091227930374576</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>

</xml_diff>